<commit_message>
Found fan header in digikey.
</commit_message>
<xml_diff>
--- a/BOM/Smart fan BOM.xlsx
+++ b/BOM/Smart fan BOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\srs\BEE484\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BEE484_SmartFan\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9523DE01-278C-4819-85A5-470AA3CBAD48}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Digikey</t>
   </si>
@@ -52,15 +53,9 @@
     <t>Arduino</t>
   </si>
   <si>
-    <t>Ebay</t>
-  </si>
-  <si>
     <t>Bracket</t>
   </si>
   <si>
-    <t>4 pin fan header x10</t>
-  </si>
-  <si>
     <t>digikey</t>
   </si>
   <si>
@@ -85,13 +80,13 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>need to find from Amazon or digikey</t>
+    <t>fan header</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,6 +149,7 @@
         <sz val="11"/>
         <color theme="10"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -171,15 +167,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F9" totalsRowCount="1">
-  <autoFilter ref="A1:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowCount="1">
+  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Link" totalsRowDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Unit price"/>
-    <tableColumn id="4" name="Quantity"/>
-    <tableColumn id="5" name="Total" totalsRowFunction="sum"/>
-    <tableColumn id="6" name="Comment"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" totalsRowDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Unit price"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quantity"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total" totalsRowFunction="sum"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -481,42 +477,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -534,7 +530,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -552,7 +548,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -570,7 +566,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -588,33 +584,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>5.5</v>
+        <v>0.46</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.3800000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C7">
         <v>2.93</v>
@@ -627,9 +620,9 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -645,25 +638,25 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
       <c r="E9">
         <f>SUBTOTAL(109,Table1[Total])</f>
-        <v>59.83</v>
+        <v>55.71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5" location="viTabs_0"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{6E9F85FF-1D23-4790-8054-7D8317E048BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
uploading version of BOM that was submitted to professor.
</commit_message>
<xml_diff>
--- a/BOM/Smart fan BOM.xlsx
+++ b/BOM/Smart fan BOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\srs\BEE484\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BEE484_SmartFan\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B62D343-FE9C-4BF8-B561-F9B1E55FDCEF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="8030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Digikey</t>
   </si>
@@ -82,15 +83,6 @@
     <t>PWM Fans x2</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>PCB Quote 100x100mm size</t>
-  </si>
-  <si>
-    <t>Qute from PCBway But unsure if that's who we'll use. Need to talk to the professor about who to give gerber files to.</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -110,13 +102,36 @@
   </si>
   <si>
     <t>8.99 Fed Ex</t>
+  </si>
+  <si>
+    <t>Elecrow</t>
+  </si>
+  <si>
+    <t>26.99  Fed Ex</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>To order from Elecrow: Default settings should be correct. But just to be sure, the settings are:
+1) Layers: 2
+2) Dimensions: 100 x 94mm (same price as 100x100)
+3) Quantity 5
+4) Different pcb design 1
+5) PCB Thickness: 1.6mm
+6) color: green
+7) surface finish: Hasl
+8) castellated hole: no
+9) Coper weight: 1oz
+10) PCB stencil: No
+Shipping: DHL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +150,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -179,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,10 +210,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,24 +531,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" customWidth="1"/>
-    <col min="9" max="9" width="25.453125" customWidth="1"/>
-    <col min="10" max="10" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -530,13 +556,13 @@
         <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
@@ -548,13 +574,13 @@
         <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -565,10 +591,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>6.99</v>
@@ -580,25 +606,25 @@
         <f>F2*G2</f>
         <v>6.99</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -607,40 +633,40 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H10" si="0">F3*G3</f>
         <v>20</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>27.51</v>
+        <v>35.770000000000003</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>27.51</v>
-      </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>35.770000000000003</v>
+      </c>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -651,10 +677,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>0.27</v>
@@ -666,11 +692,11 @@
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -681,10 +707,10 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <v>6.7</v>
@@ -696,23 +722,23 @@
         <f t="shared" si="0"/>
         <v>20.100000000000001</v>
       </c>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>0.46</v>
@@ -724,9 +750,9 @@
         <f t="shared" si="0"/>
         <v>2.7600000000000002</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -737,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>2.93</v>
@@ -752,9 +778,9 @@
         <f t="shared" si="0"/>
         <v>5.86</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -765,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>14.7</v>
@@ -780,35 +806,49 @@
         <f t="shared" si="0"/>
         <v>14.7</v>
       </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
       </c>
       <c r="F10">
-        <v>40</v>
+        <v>4.99</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>4.99</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="H11">
         <f>SUM(H2:H10)</f>
-        <v>138.46</v>
+        <v>111.71000000000001</v>
+      </c>
+      <c r="I11">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="J11" s="6">
+        <f>H11+I11</f>
+        <v>147.69</v>
       </c>
     </row>
   </sheetData>
@@ -817,16 +857,17 @@
     <mergeCell ref="I5:I9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B3" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{AFE69702-D2D2-4BE0-8D05-2DB0008CC0A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>